<commit_message>
updated kinect verification data for use in V&V doc
</commit_message>
<xml_diff>
--- a/Documents/05_ProofOfConcept/KinectTestMeasurements.xlsx
+++ b/Documents/05_ProofOfConcept/KinectTestMeasurements.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fauzi\Documents\5th Year\TRON 4TB6A\04 GIT\ModernMobility\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\School\YEAR 6\ModernMobility\Documents\05_ProofOfConcept\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3790" xr2:uid="{842DD71B-55F6-4B24-97E3-8E5E70BBF79E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="3792"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$G$2</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,9 +41,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Data #</t>
-  </si>
-  <si>
     <t>Centerline</t>
   </si>
   <si>
@@ -52,11 +49,14 @@
   <si>
     <t>Angle (max or centerline)</t>
   </si>
+  <si>
+    <t>Sample</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,15 +74,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -99,14 +105,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,7 +256,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -158,26 +269,31 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Kinect Distance vs.</a:t>
+              <a:rPr lang="en-US" b="1" u="sng"/>
+              <a:t>Kinect</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" b="1"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Expected Distance vs</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Mesaured Distance</a:t>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> Measured Distance</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Centerline</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.30463868740545363"/>
+          <c:y val="1.488095238095238E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -191,7 +307,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -209,23 +325,25 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.5392731081028669E-2"/>
+          <c:y val="0.11940792557180351"/>
+          <c:w val="0.86709398394166259"/>
+          <c:h val="0.77030078271466063"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Absolute Distance (m)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Distance Along the Centerline</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -251,9 +369,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -277,7 +395,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.49020000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74800042780736431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98802479725966397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2400326608601888</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9150065274040191</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.114007417205531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -289,15 +434,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Kinect Distance (m)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Distance Along the Max Angle</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -323,37 +460,52 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.49020000000000002</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74800042780736431</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98802479725966397</c:v>
+                  <c:v>1.1100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2400326608601888</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.9150065274040191</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.114007417205531</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$9:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5681384426352436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85755291381931642</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1342355663617678</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4104320543719928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DE19-4CFE-855B-6CBC95AD62BD}"/>
+              <c16:uniqueId val="{00000000-B34E-4BD4-AFC2-9637A2117460}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -361,21 +513,17 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Angle (max or centerline)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Expected Distance</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -385,47 +533,93 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:prstDash val="dash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="9"/>
+              <c:pt idx="0">
+                <c:v>0.25</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>0.5</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>0.75</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1.25</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>1.5</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>1.75</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>2.25</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="9"/>
+              <c:pt idx="0">
+                <c:v>0.25</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>0.5</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>0.75</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1.25</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>1.5</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>1.75</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>2.25</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-DE19-4CFE-855B-6CBC95AD62BD}"/>
+              <c16:uniqueId val="{00000001-B34E-4BD4-AFC2-9637A2117460}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -437,18 +631,76 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
         <c:axId val="453471672"/>
         <c:axId val="453472000"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="453471672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" b="1"/>
+                  <a:t>Expected Distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" b="1" baseline="0"/>
+                  <a:t> Value (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -487,11 +739,8 @@
         </c:txPr>
         <c:crossAx val="453472000"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="453472000"/>
         <c:scaling>
@@ -513,6 +762,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" b="1"/>
+                  <a:t>Measured Distance Value (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -546,7 +850,7 @@
         </c:txPr>
         <c:crossAx val="453471672"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.25"/>
         <c:minorUnit val="5.000000000000001E-2"/>
       </c:valAx>
@@ -559,7 +863,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10355403850380772"/>
+          <c:y val="0.19436789151356079"/>
+          <c:w val="0.24127354770308884"/>
+          <c:h val="0.12555891451068615"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1181,15 +1495,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>22224</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1513,251 +1827,252 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A2395B0-7B04-44BE-8A1F-46084860D2B8}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="1" max="1" width="1.77734375" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.49020000000000002</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="1">
+        <f>SQRT(F4^2 +G4^2)</f>
+        <v>0.74800042780736431</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.748</v>
+      </c>
+      <c r="G4" s="6">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
+      <c r="D5" s="1">
+        <f>SQRT(F5^2 +G5^2)</f>
+        <v>0.98802479725966397</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="G5" s="6">
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0.5</v>
-      </c>
-      <c r="C2">
-        <v>0.49020000000000002</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="D6" s="1">
+        <f>SQRT(F6^2 +G6^2)</f>
+        <v>1.2400326608601888</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="G6" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="5">
         <v>5</v>
       </c>
+      <c r="C7" s="1">
+        <v>1.92</v>
+      </c>
+      <c r="D7" s="1">
+        <f>SQRT(F7^2 +G7^2)</f>
+        <v>1.9150065274040191</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.915</v>
+      </c>
+      <c r="G7" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0.75</v>
-      </c>
-      <c r="C3">
-        <f>SQRT(E3^2 +F3^2)</f>
-        <v>0.74800042780736431</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>0.748</v>
-      </c>
-      <c r="F3">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f>SQRT(E4^2 +F4^2)</f>
-        <v>0.98802479725966397</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="F4">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1.25</v>
-      </c>
-      <c r="C5">
-        <f>SQRT(E5^2 +F5^2)</f>
-        <v>1.2400326608601888</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>1.24</v>
-      </c>
-      <c r="F5">
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1.92</v>
-      </c>
-      <c r="C6">
-        <f>SQRT(E6^2 +F6^2)</f>
-        <v>1.9150065274040191</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.915</v>
-      </c>
-      <c r="F6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="5">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C8" s="1">
         <f>1.92+0.21</f>
         <v>2.13</v>
       </c>
-      <c r="C7">
-        <f>SQRT(E7^2 +F7^2)</f>
+      <c r="D8" s="1">
+        <f>SQRT(F8^2 +G8^2)</f>
         <v>2.114007417205531</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.1139999999999999</v>
+      </c>
+      <c r="G8" s="6">
+        <v>5.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="5">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D9" s="1">
+        <f>SQRT(F9^2 +G9^2)</f>
+        <v>0.5681384426352436</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E7">
-        <v>2.1139999999999999</v>
-      </c>
-      <c r="F7">
-        <v>5.5999999999999999E-3</v>
+      <c r="F9" s="1">
+        <v>0.49769999999999998</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.54</v>
-      </c>
-      <c r="C8">
-        <f>SQRT(E8^2 +F8^2)</f>
-        <v>0.5681384426352436</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>0.49769999999999998</v>
-      </c>
-      <c r="F8">
-        <v>0.27400000000000002</v>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D10" s="1">
+        <f>SQRT(F10^2 +G10^2)</f>
+        <v>0.85755291381931642</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.751</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0.84</v>
-      </c>
-      <c r="C9">
-        <f>SQRT(E9^2 +F9^2)</f>
-        <v>0.85755291381931642</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>0.751</v>
-      </c>
-      <c r="F9">
-        <v>0.41399999999999998</v>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="5">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <f>SQRT(F11^2 +G11^2)</f>
+        <v>1.1342355663617678</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.99339999999999995</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.5474</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C10">
-        <f>SQRT(E10^2 +F10^2)</f>
-        <v>1.1342355663617678</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10">
-        <v>0.99339999999999995</v>
-      </c>
-      <c r="F10">
-        <v>0.5474</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="12" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="7">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C12" s="8">
         <v>1.4</v>
       </c>
-      <c r="C11">
-        <f>SQRT(E11^2 +F11^2)</f>
+      <c r="D12" s="8">
+        <f>SQRT(F12^2 +G12^2)</f>
         <v>1.4104320543719928</v>
       </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11">
+      <c r="E12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="8">
         <v>1.2353000000000001</v>
       </c>
-      <c r="F11">
+      <c r="G12" s="9">
         <v>0.68069999999999997</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F1" xr:uid="{232B202D-B3D7-4B18-BB14-33E549B7B016}">
-    <sortState ref="B2:F11">
-      <sortCondition ref="D1"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>